<commit_message>
add row for GRCh37_test featureset
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_sample.xlsx
+++ b/inst/extdata/scidb_metadata_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/revealgenomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D89295D-954B-0B4B-9F0B-9233E572294A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC5DDCE-0E86-0F40-8C4F-631BB4C13AA5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XLS version" sheetId="23" r:id="rId1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="492">
   <si>
     <t>sample_name</t>
   </si>
@@ -1698,6 +1698,9 @@
   </si>
   <si>
     <t>project_owner_email</t>
+  </si>
+  <si>
+    <t>GRCh37_test</t>
   </si>
 </sst>
 </file>
@@ -4257,11 +4260,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4738,6 +4741,23 @@
         <v>150</v>
       </c>
       <c r="E27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>491</v>
+      </c>
+      <c r="B28" t="s">
+        <v>491</v>
+      </c>
+      <c r="C28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
         <v>149</v>
       </c>
     </row>
@@ -10961,7 +10981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Y1" sqref="Y1"/>
     </sheetView>
@@ -34897,9 +34917,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2:M11"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34991,7 +35011,7 @@
         <v>999</v>
       </c>
       <c r="I2" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>488</v>
@@ -35027,7 +35047,7 @@
         <v>999</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>488</v>
@@ -35063,7 +35083,7 @@
         <v>999</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>488</v>
@@ -35099,7 +35119,7 @@
         <v>999</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>488</v>
@@ -35138,7 +35158,7 @@
         <v>999</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>488</v>
@@ -35177,7 +35197,7 @@
         <v>999</v>
       </c>
       <c r="I7" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>488</v>
@@ -35216,7 +35236,7 @@
         <v>999</v>
       </c>
       <c r="I8" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>488</v>
@@ -35255,7 +35275,7 @@
         <v>999</v>
       </c>
       <c r="I9" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>488</v>
@@ -35294,7 +35314,7 @@
         <v>999</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>488</v>
@@ -35333,7 +35353,7 @@
         <v>999</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>180</v>
+        <v>491</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>488</v>

</xml_diff>

<commit_message>
add data and excel file links for Tophat Fusion
- add data file with 3 samples worth of data
- Excel file
    + add new samples to Sample sheet
    + add rows for new file in Pipelines sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_sample.xlsx
+++ b/inst/extdata/scidb_metadata_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/revealgenomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC5DDCE-0E86-0F40-8C4F-631BB4C13AA5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30658BA-9B77-FC4E-B284-BC051F87C743}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XLS version" sheetId="23" r:id="rId1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="497">
   <si>
     <t>sample_name</t>
   </si>
@@ -1701,6 +1701,21 @@
   </si>
   <si>
     <t>GRCh37_test</t>
+  </si>
+  <si>
+    <t>[external]-[Fusion] Tophat Fusion</t>
+  </si>
+  <si>
+    <t>data_study_a_TophatFusion_Results.txt</t>
+  </si>
+  <si>
+    <t>s003_2</t>
+  </si>
+  <si>
+    <t>s003_3</t>
+  </si>
+  <si>
+    <t>visit_3</t>
   </si>
 </sst>
 </file>
@@ -2110,7 +2125,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2188,6 +2203,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4262,7 +4278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
@@ -10981,7 +10997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Y1" sqref="Y1"/>
     </sheetView>
@@ -13086,9 +13102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AX1518"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13575,14 +13591,55 @@
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="41"/>
-      <c r="K6" s="23"/>
-      <c r="O6" s="41"/>
-      <c r="Q6" s="2"/>
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>475</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>CONCATENATE(F6,"__",J6)</f>
+        <v>s003_2__DNA</v>
+      </c>
+      <c r="F6" t="s">
+        <v>494</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>441</v>
+      </c>
+      <c r="J6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="L6" t="s">
+        <v>443</v>
+      </c>
+      <c r="M6" t="s">
+        <v>444</v>
+      </c>
+      <c r="N6" t="s">
+        <v>316</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>441</v>
+      </c>
+      <c r="P6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>379</v>
+      </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -13600,16 +13657,69 @@
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
+      <c r="AJ6" t="s">
+        <v>471</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>477</v>
+      </c>
+      <c r="AL6" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="41"/>
-      <c r="K7" s="23"/>
-      <c r="O7" s="41"/>
-      <c r="Q7" s="2"/>
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>475</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f>CONCATENATE(F7,"__",J7)</f>
+        <v>s003_3__DNA</v>
+      </c>
+      <c r="F7" t="s">
+        <v>495</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="I7" s="41" t="s">
+        <v>441</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="L7" t="s">
+        <v>443</v>
+      </c>
+      <c r="M7" t="s">
+        <v>444</v>
+      </c>
+      <c r="N7" t="s">
+        <v>316</v>
+      </c>
+      <c r="O7" s="41" t="s">
+        <v>441</v>
+      </c>
+      <c r="P7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>379</v>
+      </c>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
@@ -13627,6 +13737,18 @@
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
+      <c r="AJ7" t="s">
+        <v>471</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>477</v>
+      </c>
+      <c r="AL7" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
@@ -34915,11 +35037,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35363,6 +35485,114 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6" t="s">
         <v>487</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="40">
+        <v>1</v>
+      </c>
+      <c r="C12" s="40">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" ref="D12" si="1">CONCATENATE(E12,"__DNA")</f>
+        <v>s001_1__DNA</v>
+      </c>
+      <c r="E12" t="s">
+        <v>480</v>
+      </c>
+      <c r="F12" t="s">
+        <v>492</v>
+      </c>
+      <c r="G12" t="s">
+        <v>280</v>
+      </c>
+      <c r="H12" s="6">
+        <v>2</v>
+      </c>
+      <c r="I12" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="N12" s="45" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="40">
+        <v>1</v>
+      </c>
+      <c r="C13" s="40">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f t="shared" ref="D13:D14" si="2">CONCATENATE(E13,"__DNA")</f>
+        <v>s001_1__DNA</v>
+      </c>
+      <c r="E13" t="s">
+        <v>480</v>
+      </c>
+      <c r="F13" t="s">
+        <v>492</v>
+      </c>
+      <c r="G13" t="s">
+        <v>280</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="N13" s="45" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>1</v>
+      </c>
+      <c r="B14" s="40">
+        <v>1</v>
+      </c>
+      <c r="C14" s="40">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>s001_1__DNA</v>
+      </c>
+      <c r="E14" t="s">
+        <v>480</v>
+      </c>
+      <c r="F14" t="s">
+        <v>492</v>
+      </c>
+      <c r="G14" t="s">
+        <v>280</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="N14" s="45" t="s">
+        <v>493</v>
       </c>
     </row>
   </sheetData>
@@ -35389,7 +35619,7 @@
           <x14:formula1>
             <xm:f>pipeline_choices!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F2:F11 F15:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA976312-A594-4F1B-911A-2078BC9B4731}">
           <x14:formula1>
@@ -35401,7 +35631,7 @@
           <x14:formula1>
             <xm:f>filter_choices!$B$2:$B$36</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>G2:G11 G15:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -35476,7 +35706,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add more data and excel file links for Tophat Fusion
- add 3 per sample files of Tophat Fusion data
- Excel file
    + add second study to Study sheet
    + add new subjects, samples for the new study
    + add rows for Tophat fusion in Pipelines sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_sample.xlsx
+++ b/inst/extdata/scidb_metadata_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/revealgenomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30658BA-9B77-FC4E-B284-BC051F87C743}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EB8B30-7B8F-6A49-AADD-6277B374472A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XLS version" sheetId="23" r:id="rId1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="519">
   <si>
     <t>sample_name</t>
   </si>
@@ -1716,6 +1716,72 @@
   </si>
   <si>
     <t>visit_3</t>
+  </si>
+  <si>
+    <t>data_study_b_1004_L1.D443.tophat.fusions.filtered.txt</t>
+  </si>
+  <si>
+    <t>sample_study_b</t>
+  </si>
+  <si>
+    <t>sample_project_a_sample_study_b</t>
+  </si>
+  <si>
+    <t>https://clinicaltrials.gov/ct2/show/yyyy</t>
+  </si>
+  <si>
+    <t>Jack Barker</t>
+  </si>
+  <si>
+    <t>study_b_3045</t>
+  </si>
+  <si>
+    <t>study_b_3045_subj1004</t>
+  </si>
+  <si>
+    <t>s1004</t>
+  </si>
+  <si>
+    <t>multiple myeloma</t>
+  </si>
+  <si>
+    <t>study_b_3045_subj1022</t>
+  </si>
+  <si>
+    <t>s1022</t>
+  </si>
+  <si>
+    <t>study_b_3045_subj1058</t>
+  </si>
+  <si>
+    <t>s1058</t>
+  </si>
+  <si>
+    <t>1004_L1.D443</t>
+  </si>
+  <si>
+    <t>tissue</t>
+  </si>
+  <si>
+    <t>RELAPSE</t>
+  </si>
+  <si>
+    <t>1004_L2.D443</t>
+  </si>
+  <si>
+    <t>1022_L1.D354</t>
+  </si>
+  <si>
+    <t>1058_L3.D125</t>
+  </si>
+  <si>
+    <t>GRCh38_test</t>
+  </si>
+  <si>
+    <t>data_study_b_1022_L1.D354.tophat.fusions.filtered.txt</t>
+  </si>
+  <si>
+    <t>data_study_b_1058_L3.D125.tophat.fusions.filtered.txt</t>
   </si>
 </sst>
 </file>
@@ -1835,7 +1901,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1893,6 +1959,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2125,7 +2197,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2204,6 +2276,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4276,11 +4352,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4573,7 +4649,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>157</v>
       </c>
@@ -4590,7 +4666,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -4607,7 +4683,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>158</v>
       </c>
@@ -4624,7 +4700,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -4641,7 +4717,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>159</v>
       </c>
@@ -4658,7 +4734,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -4675,7 +4751,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>161</v>
       </c>
@@ -4692,7 +4768,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>162</v>
       </c>
@@ -4709,7 +4785,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>288</v>
       </c>
@@ -4726,7 +4802,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>163</v>
       </c>
@@ -4743,7 +4819,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>287</v>
       </c>
@@ -4760,7 +4836,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>491</v>
       </c>
@@ -4776,6 +4852,24 @@
       <c r="E28" t="s">
         <v>149</v>
       </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>516</v>
+      </c>
+      <c r="B29" t="s">
+        <v>516</v>
+      </c>
+      <c r="C29" t="s">
+        <v>174</v>
+      </c>
+      <c r="D29">
+        <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" s="19"/>
     </row>
   </sheetData>
   <sortState ref="B7:F26">
@@ -10995,11 +11089,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11152,12 +11246,76 @@
         <v>469</v>
       </c>
     </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q3" s="38" t="s">
+        <v>500</v>
+      </c>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="V3" s="39" t="s">
+        <v>468</v>
+      </c>
+      <c r="W3" s="38" t="s">
+        <v>469</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="Q2" r:id="rId1" xr:uid="{E704E98C-8FCD-4FD9-AB84-8A168AF35D93}"/>
     <hyperlink ref="W2" r:id="rId2" xr:uid="{61C0B8F2-1015-453F-8D53-78B5DBD873D7}"/>
+    <hyperlink ref="Q3" r:id="rId3" xr:uid="{BCC24955-1D00-174F-8CA7-43EAF241F0A3}"/>
+    <hyperlink ref="W3" r:id="rId4" xr:uid="{6FEBE100-25D8-2D40-A608-B2DC6F944976}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -11167,7 +11325,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:H2"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11286,22 +11444,82 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="40">
+        <v>1</v>
+      </c>
+      <c r="C5" s="40">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1004</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="F5" t="s">
+        <v>502</v>
+      </c>
+      <c r="G5" t="s">
+        <v>503</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="E6" s="41"/>
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="40">
+        <v>1</v>
+      </c>
+      <c r="C6" s="40">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1022</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="F6" t="s">
+        <v>502</v>
+      </c>
+      <c r="G6" t="s">
+        <v>506</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="40">
+        <v>1</v>
+      </c>
+      <c r="C7" s="40">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1058</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="F7" t="s">
+        <v>502</v>
+      </c>
+      <c r="G7" t="s">
+        <v>508</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
@@ -13102,9 +13320,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AX1518"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="F10" activeCellId="1" sqref="D10:D11 F10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13258,7 +13476,9 @@
       <c r="AM1" t="s">
         <v>442</v>
       </c>
-      <c r="AN1"/>
+      <c r="AN1" t="s">
+        <v>512</v>
+      </c>
       <c r="AO1"/>
       <c r="AP1"/>
       <c r="AQ1"/>
@@ -13751,14 +13971,55 @@
       </c>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="41"/>
-      <c r="K8" s="23"/>
-      <c r="O8" s="41"/>
-      <c r="Q8" s="2"/>
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>1004</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f>CONCATENATE(F8,"__",J8)</f>
+        <v>1004_L1.D443__DNA</v>
+      </c>
+      <c r="F8" t="s">
+        <v>510</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="L8" t="s">
+        <v>443</v>
+      </c>
+      <c r="M8" t="s">
+        <v>444</v>
+      </c>
+      <c r="N8" t="s">
+        <v>316</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="P8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>379</v>
+      </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
@@ -13776,16 +14037,70 @@
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
+      <c r="AJ8" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>503</v>
+      </c>
+      <c r="AL8" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="AM8" s="5"/>
+      <c r="AN8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="41"/>
-      <c r="K9" s="23"/>
-      <c r="O9" s="41"/>
-      <c r="Q9" s="2"/>
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1004</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f>CONCATENATE(F9,"__",J9)</f>
+        <v>1004_L2.D443__DNA</v>
+      </c>
+      <c r="F9" t="s">
+        <v>513</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="L9" t="s">
+        <v>443</v>
+      </c>
+      <c r="M9" t="s">
+        <v>444</v>
+      </c>
+      <c r="N9" t="s">
+        <v>316</v>
+      </c>
+      <c r="O9" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="P9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>379</v>
+      </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
@@ -13803,16 +14118,69 @@
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
+      <c r="AJ9" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>503</v>
+      </c>
+      <c r="AL9" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="AN9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="41"/>
-      <c r="K10" s="23"/>
-      <c r="O10" s="41"/>
-      <c r="Q10" s="2"/>
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="40">
+        <v>1</v>
+      </c>
+      <c r="C10" s="40">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1022</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f>CONCATENATE(F10,"__",J10)</f>
+        <v>1022_L1.D354__DNA</v>
+      </c>
+      <c r="F10" t="s">
+        <v>514</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="L10" t="s">
+        <v>443</v>
+      </c>
+      <c r="M10" t="s">
+        <v>444</v>
+      </c>
+      <c r="N10" t="s">
+        <v>316</v>
+      </c>
+      <c r="O10" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="P10" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>379</v>
+      </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -13830,16 +14198,69 @@
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
+      <c r="AJ10" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>506</v>
+      </c>
+      <c r="AL10" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="41"/>
-      <c r="K11" s="23"/>
-      <c r="O11" s="41"/>
-      <c r="Q11" s="2"/>
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" s="40">
+        <v>1</v>
+      </c>
+      <c r="C11" s="40">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>1058</v>
+      </c>
+      <c r="E11" s="2" t="str">
+        <f>CONCATENATE(F11,"__",J11)</f>
+        <v>1058_L3.D125__DNA</v>
+      </c>
+      <c r="F11" t="s">
+        <v>515</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="L11" t="s">
+        <v>443</v>
+      </c>
+      <c r="M11" t="s">
+        <v>444</v>
+      </c>
+      <c r="N11" t="s">
+        <v>316</v>
+      </c>
+      <c r="O11" s="41" t="s">
+        <v>505</v>
+      </c>
+      <c r="P11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>379</v>
+      </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
@@ -13857,6 +14278,18 @@
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
+      <c r="AJ11" t="s">
+        <v>502</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>508</v>
+      </c>
+      <c r="AL11" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
@@ -35037,11 +35470,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35593,6 +36026,111 @@
       </c>
       <c r="N14" s="45" t="s">
         <v>493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="46">
+        <v>1</v>
+      </c>
+      <c r="B15" s="47">
+        <v>1</v>
+      </c>
+      <c r="C15" s="47">
+        <v>2</v>
+      </c>
+      <c r="D15" s="48">
+        <v>1004</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>510</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>492</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="H15" s="46">
+        <v>1</v>
+      </c>
+      <c r="I15" s="48" t="s">
+        <v>516</v>
+      </c>
+      <c r="J15" s="46" t="s">
+        <v>488</v>
+      </c>
+      <c r="N15" s="49" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="40">
+        <v>1</v>
+      </c>
+      <c r="C16" s="40">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1022</v>
+      </c>
+      <c r="E16" t="s">
+        <v>514</v>
+      </c>
+      <c r="F16" t="s">
+        <v>492</v>
+      </c>
+      <c r="G16" t="s">
+        <v>280</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>1</v>
+      </c>
+      <c r="B17" s="40">
+        <v>1</v>
+      </c>
+      <c r="C17" s="40">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1058</v>
+      </c>
+      <c r="E17" t="s">
+        <v>515</v>
+      </c>
+      <c r="F17" t="s">
+        <v>492</v>
+      </c>
+      <c r="G17" t="s">
+        <v>280</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -35619,7 +36157,7 @@
           <x14:formula1>
             <xm:f>pipeline_choices!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F11 F15:F1048576</xm:sqref>
+          <xm:sqref>F2:F11 F18:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA976312-A594-4F1B-911A-2078BC9B4731}">
           <x14:formula1>
@@ -35631,7 +36169,7 @@
           <x14:formula1>
             <xm:f>filter_choices!$B$2:$B$36</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G11 G15:G1048576</xm:sqref>
+          <xm:sqref>G2:G11 G18:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add data and excel file links for Defuse Fusion
- add 2 per sample files of Tophat Fusion data
- Excel file
    + add rows for Defuse fusion in Pipelines sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_sample.xlsx
+++ b/inst/extdata/scidb_metadata_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/revealgenomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EB8B30-7B8F-6A49-AADD-6277B374472A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE42CA8F-C910-244C-B0D8-9351014D7821}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XLS version" sheetId="23" r:id="rId1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="522">
   <si>
     <t>sample_name</t>
   </si>
@@ -1782,6 +1782,15 @@
   </si>
   <si>
     <t>data_study_b_1058_L3.D125.tophat.fusions.filtered.txt</t>
+  </si>
+  <si>
+    <t>[external]-[Fusion] Defuse</t>
+  </si>
+  <si>
+    <t>data_study_b_1004_L1.D443.defuse.results.filtered.tsv</t>
+  </si>
+  <si>
+    <t>data_study_b_1022_L1.D354.defuse.results.filtered.tsv</t>
   </si>
 </sst>
 </file>
@@ -1901,7 +1910,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1965,6 +1974,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2197,7 +2212,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2280,6 +2295,7 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -13320,7 +13336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AX1518"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F10" activeCellId="1" sqref="D10:D11 F10:F11"/>
     </sheetView>
@@ -35470,9 +35486,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
@@ -36044,7 +36060,7 @@
       <c r="E15" s="48" t="s">
         <v>510</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="50" t="s">
         <v>492</v>
       </c>
       <c r="G15" s="48" t="s">
@@ -36079,7 +36095,7 @@
       <c r="E16" t="s">
         <v>514</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="50" t="s">
         <v>492</v>
       </c>
       <c r="G16" t="s">
@@ -36114,7 +36130,7 @@
       <c r="E17" t="s">
         <v>515</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="50" t="s">
         <v>492</v>
       </c>
       <c r="G17" t="s">
@@ -36131,6 +36147,76 @@
       </c>
       <c r="N17" s="1" t="s">
         <v>518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>1</v>
+      </c>
+      <c r="B18" s="40">
+        <v>1</v>
+      </c>
+      <c r="C18" s="40">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1004</v>
+      </c>
+      <c r="E18" t="s">
+        <v>510</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>519</v>
+      </c>
+      <c r="G18" t="s">
+        <v>280</v>
+      </c>
+      <c r="H18" s="6">
+        <v>2</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>1</v>
+      </c>
+      <c r="B19" s="40">
+        <v>1</v>
+      </c>
+      <c r="C19" s="40">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1004</v>
+      </c>
+      <c r="E19" t="s">
+        <v>514</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>519</v>
+      </c>
+      <c r="G19" t="s">
+        <v>280</v>
+      </c>
+      <c r="H19" s="6">
+        <v>2</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -36169,7 +36255,7 @@
           <x14:formula1>
             <xm:f>filter_choices!$B$2:$B$36</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G11 G18:G1048576</xm:sqref>
+          <xm:sqref>G2:G11 G20:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
fix bugs in sample excel sheet
- sample naming errors were fixed
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_sample.xlsx
+++ b/inst/extdata/scidb_metadata_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/revealgenomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE42CA8F-C910-244C-B0D8-9351014D7821}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D64CB8-7FC5-CD4D-8FDB-F259F48AAB3F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="14240" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Definitions!$A$1:$O$168</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">pipeline_choices!$B$1:$M$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Pipelines!$A$1:$N$4580</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Pipelines!$A$1:$N$4579</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Samples!$A$1:$AH$1518</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Subjects!$A$1:$E$1068</definedName>
   </definedNames>
@@ -2513,24 +2513,6 @@
     <cellStyle name="XLConnect.String" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
   </cellStyles>
   <dxfs count="87">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3391,6 +3373,24 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -4052,7 +4052,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B1:B1048576" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B1:B1048576" totalsRowShown="0" headerRowDxfId="86">
   <autoFilter ref="B1:B1048576" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="featureset_scidb"/>
@@ -10759,174 +10759,174 @@
   </sheetData>
   <autoFilter ref="A1:O168" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="H169:O1048576 O25:O29 N40:O42 H40:L42 H25:K36 N30:O36 O102:O168 H102:M168 N64:O66 H64:L66 M38:M42 N38:O38 H38:L38 L56:M56 M64:M67 H51:O53 H2:O9 L11:M36 N11:N29 O11:O23 H11:K23 H59:O62 H68:O78">
-    <cfRule type="containsText" dxfId="86" priority="104" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="85" priority="104" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="105" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="84" priority="105" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F169:F1048576 F40:F42 F25:F36 F38 F51:F52 F1:F23 F56 F59:F62 F64:F120">
-    <cfRule type="cellIs" dxfId="84" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="103" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:K24 O24">
-    <cfRule type="containsText" dxfId="83" priority="98" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="82" priority="98" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="99" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="81" priority="99" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="81" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="97" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F121:F132">
-    <cfRule type="cellIs" dxfId="80" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="94" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F133:F144">
-    <cfRule type="cellIs" dxfId="79" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="93" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F145:F156">
-    <cfRule type="cellIs" dxfId="78" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="92" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F157:F168">
-    <cfRule type="cellIs" dxfId="77" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="91" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N102:N168">
-    <cfRule type="containsText" dxfId="76" priority="89" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="75" priority="89" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",N102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="90" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="74" priority="90" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",N102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56:K56 O56">
-    <cfRule type="containsText" dxfId="74" priority="87" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="73" priority="87" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="88" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="72" priority="88" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="containsText" dxfId="72" priority="85" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="71" priority="85" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",N56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="86" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="70" priority="86" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",N56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:L39 N39:O39">
-    <cfRule type="containsText" dxfId="70" priority="61" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="69" priority="61" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="62" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="68" priority="62" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39">
-    <cfRule type="cellIs" dxfId="68" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="60" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67:L67 N67:O67">
-    <cfRule type="containsText" dxfId="67" priority="58" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="66" priority="58" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H67)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="59" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="65" priority="59" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:O44 H47:O50">
-    <cfRule type="containsText" dxfId="65" priority="54" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="64" priority="54" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="55" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:F44 F47:F50">
-    <cfRule type="cellIs" dxfId="63" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="53" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:O46">
-    <cfRule type="containsText" dxfId="62" priority="51" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="61" priority="51" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="52" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="60" priority="52" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:F46">
-    <cfRule type="cellIs" dxfId="60" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54:O55">
-    <cfRule type="containsText" dxfId="59" priority="48" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="58" priority="48" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="49" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="57" priority="49" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:F55">
-    <cfRule type="cellIs" dxfId="57" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="47" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O97 H97:M97">
-    <cfRule type="containsText" dxfId="56" priority="45" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="55" priority="45" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="46" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="54" priority="46" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N97">
-    <cfRule type="containsText" dxfId="54" priority="43" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="53" priority="43" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",N97)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="44" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="52" priority="44" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",N97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63:O63">
-    <cfRule type="containsText" dxfId="52" priority="41" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="51" priority="41" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="42" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="50" priority="42" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63">
-    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37:O37">
-    <cfRule type="containsText" dxfId="49" priority="37" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="48" priority="37" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="38" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="47" priority="38" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37">
-    <cfRule type="cellIs" dxfId="47" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10940,7 +10940,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53">
-    <cfRule type="cellIs" dxfId="46" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10954,10 +10954,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:O10">
-    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="43" priority="26" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H10)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10971,15 +10971,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:O55">
-    <cfRule type="containsText" dxfId="43" priority="22" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="23" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55">
-    <cfRule type="cellIs" dxfId="41" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10993,31 +10993,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57:F58">
-    <cfRule type="cellIs" dxfId="40" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57:M58">
-    <cfRule type="containsText" dxfId="39" priority="17" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="38" priority="17" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",L57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="18" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",L57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:K58 O57:O58">
-    <cfRule type="containsText" dxfId="37" priority="15" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="16" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57:N58">
-    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="34" priority="13" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",N57)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="33" priority="14" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",N57)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11031,10 +11031,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79:O96">
-    <cfRule type="containsText" dxfId="33" priority="10" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="32" priority="10" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H79)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="11" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="31" priority="11" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H79)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11057,18 +11057,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O98:O100 H98:M100">
-    <cfRule type="containsText" dxfId="31" priority="8" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H98)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H98)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N98:N100">
-    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",N98)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",N98)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11082,18 +11082,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O101 H101:M101">
-    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",H101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="25" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H101)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N101">
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",N101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",N101)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35488,9 +35488,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35984,10 +35984,10 @@
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" ref="D13:D14" si="2">CONCATENATE(E13,"__DNA")</f>
-        <v>s001_1__DNA</v>
+        <v>s003_1__DNA</v>
       </c>
       <c r="E13" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="F13" t="s">
         <v>492</v>
@@ -36020,10 +36020,10 @@
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>s001_1__DNA</v>
+        <v>s003_2__DNA</v>
       </c>
       <c r="E14" t="s">
-        <v>480</v>
+        <v>494</v>
       </c>
       <c r="F14" t="s">
         <v>492</v>
@@ -36049,10 +36049,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="48">
         <v>1004</v>
@@ -36084,10 +36084,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>1022</v>
@@ -36119,10 +36119,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>1058</v>
@@ -36154,10 +36154,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>1004</v>
@@ -36189,13 +36189,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>1004</v>
+        <v>1022</v>
       </c>
       <c r="E19" t="s">
         <v>514</v>
@@ -36220,13 +36220,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N4580" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
-  <sortState ref="A2:N4580">
-    <sortCondition ref="F2:F4580"/>
-    <sortCondition ref="A2:A4580"/>
-    <sortCondition ref="B2:B4580"/>
-    <sortCondition ref="C2:C4580"/>
-    <sortCondition ref="D2:D4580"/>
+  <sortState ref="A2:N4579">
+    <sortCondition ref="F2:F4579"/>
+    <sortCondition ref="A2:A4579"/>
+    <sortCondition ref="B2:B4579"/>
+    <sortCondition ref="C2:C4579"/>
+    <sortCondition ref="D2:D4579"/>
   </sortState>
   <dataConsolidate/>
   <dataValidations count="1">
@@ -36245,17 +36244,17 @@
           </x14:formula1>
           <xm:sqref>F2:F11 F18:F1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000002000000}">
+          <x14:formula1>
+            <xm:f>filter_choices!$B$2:$B$36</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G11 G20:G1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA976312-A594-4F1B-911A-2078BC9B4731}">
           <x14:formula1>
             <xm:f>featureset_choices!$A$2:$A$30</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000002000000}">
-          <x14:formula1>
-            <xm:f>filter_choices!$B$2:$B$36</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G11 G20:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -36330,7 +36329,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37524,99 +37523,99 @@
   </sheetData>
   <autoFilter ref="B1:M30" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <conditionalFormatting sqref="K26:L28 K31:L31 K35:L1048576 K2:L23">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="27" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24:L24">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29:L29">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:L30">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26:H31 H35:H1048576 H2:H24">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:A31 A35:A1048576 A1:A24">
-    <cfRule type="duplicateValues" dxfId="18" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:A20">
-    <cfRule type="duplicateValues" dxfId="17" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A14">
-    <cfRule type="duplicateValues" dxfId="16" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25:L25">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:L32">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:L33">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:L34">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A8">
-    <cfRule type="duplicateValues" dxfId="2" priority="148"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="148"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A8">
-    <cfRule type="duplicateValues" dxfId="1" priority="149"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="149"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -37631,7 +37630,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
rectify incorrect sample_name entry in Pipelines sheet
- for study 2, sample was "1022" when it should have been "1022_L1.xxx__DNA" and so on
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_sample.xlsx
+++ b/inst/extdata/scidb_metadata_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/revealgenomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C9263F-C6AF-6042-96A5-23D8FBA9E07D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D466A4-4BF6-1A4A-94AE-AA72EF1440B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -2652,7 +2652,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2987,7 +2987,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3309,7 +3309,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3476,7 +3476,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -12428,7 +12428,7 @@
         <v>10</v>
       </c>
       <c r="G98" s="31">
-        <f t="shared" ref="G98:G129" si="3">IF(COUNTIF(H98:O98,"TRUE")&gt;0,1,0)</f>
+        <f t="shared" ref="G98:G101" si="3">IF(COUNTIF(H98:O98,"TRUE")&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="H98" s="32" t="b">
@@ -14203,7 +14203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -17807,7 +17807,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:IV314"/>
   <sheetViews>
-    <sheetView defaultGridColor="0" colorId="12" workbookViewId="0"/>
+    <sheetView defaultGridColor="0" colorId="12" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20422,7 +20424,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:IV19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20497,7 +20501,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="25" t="str">
-        <f t="shared" ref="D2:D14" si="0">CONCATENATE(E2,"__DNA")</f>
+        <f t="shared" ref="D2:D19" si="0">CONCATENATE(E2,"__DNA")</f>
         <v>s001_1__DNA</v>
       </c>
       <c r="E2" s="45" t="s">
@@ -21003,8 +21007,9 @@
       <c r="C15" s="75">
         <v>1</v>
       </c>
-      <c r="D15" s="75">
-        <v>1004</v>
+      <c r="D15" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>1004_L1.D443__DNA</v>
       </c>
       <c r="E15" s="63" t="s">
         <v>299</v>
@@ -21041,8 +21046,9 @@
       <c r="C16" s="24">
         <v>1</v>
       </c>
-      <c r="D16" s="24">
-        <v>1022</v>
+      <c r="D16" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>1022_L1.D354__DNA</v>
       </c>
       <c r="E16" s="45" t="s">
         <v>302</v>
@@ -21079,8 +21085,9 @@
       <c r="C17" s="32">
         <v>1</v>
       </c>
-      <c r="D17" s="32">
-        <v>1058</v>
+      <c r="D17" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>1058_L3.D125__DNA</v>
       </c>
       <c r="E17" s="47" t="s">
         <v>303</v>
@@ -21117,8 +21124,9 @@
       <c r="C18" s="32">
         <v>1</v>
       </c>
-      <c r="D18" s="32">
-        <v>1004</v>
+      <c r="D18" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>1004_L1.D443__DNA</v>
       </c>
       <c r="E18" s="47" t="s">
         <v>299</v>
@@ -21155,8 +21163,9 @@
       <c r="C19" s="32">
         <v>1</v>
       </c>
-      <c r="D19" s="32">
-        <v>1022</v>
+      <c r="D19" s="70" t="str">
+        <f t="shared" si="0"/>
+        <v>1022_L1.D354__DNA</v>
       </c>
       <c r="E19" s="47" t="s">
         <v>302</v>
@@ -21428,7 +21437,7 @@
     </row>
     <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E2,"PharmaCompanyX_",""),"]-[",C2,"] ",D2)</f>
+        <f t="shared" ref="A2:A20" si="0">CONCATENATE("[",SUBSTITUTE(E2,"PharmaCompanyX_",""),"]-[",C2,"] ",D2)</f>
         <v>[external]-[Exome CNV] CBS - Circular Binary Segmentation</v>
       </c>
       <c r="B2" s="88" t="s">
@@ -21464,7 +21473,7 @@
     </row>
     <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E3,"PharmaCompanyX_",""),"]-[",C3,"] ",D3)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Exome CNV] HMM - hidden Markov model</v>
       </c>
       <c r="B3" s="90" t="s">
@@ -21500,7 +21509,7 @@
     </row>
     <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E4,"PharmaCompanyX_",""),"]-[",C4,"] ",D4)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Exome CNV] custom pipeline - Foundation Medicine</v>
       </c>
       <c r="B4" s="90" t="s">
@@ -21534,7 +21543,7 @@
     </row>
     <row r="5" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E5,"PharmaCompanyX_",""),"]-[",C5,"] ",D5)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Whole Genome CNV] CBS - Circular Binary Segmentation</v>
       </c>
       <c r="B5" s="90" t="s">
@@ -21570,7 +21579,7 @@
     </row>
     <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E6,"PharmaCompanyX_",""),"]-[",C6,"] ",D6)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Whole Genome CNV] HMM - hidden Markov model</v>
       </c>
       <c r="B6" s="90" t="s">
@@ -21606,7 +21615,7 @@
     </row>
     <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E7,"PharmaCompanyX_",""),"]-[",C7,"] ",D7)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Single Nucleotide Variant] MuTect / seurat / strelka</v>
       </c>
       <c r="B7" s="90" t="s">
@@ -21640,7 +21649,7 @@
     </row>
     <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E8,"PharmaCompanyX_",""),"]-[",C8,"] ",D8)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Single Nucleotide Variant] custom pipeline - Foundation Medicine</v>
       </c>
       <c r="B8" s="90" t="s">
@@ -21676,7 +21685,7 @@
     </row>
     <row r="9" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E9,"PharmaCompanyX_",""),"]-[",C9,"] ",D9)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[RNA-seq] Cufflinks</v>
       </c>
       <c r="B9" s="90" t="s">
@@ -21710,7 +21719,7 @@
     </row>
     <row r="10" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E10,"PharmaCompanyX_",""),"]-[",C10,"] ",D10)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[RNA-seq] HTSeq</v>
       </c>
       <c r="B10" s="90" t="s">
@@ -21744,7 +21753,7 @@
     </row>
     <row r="11" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E11,"PharmaCompanyX_",""),"]-[",C11,"] ",D11)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[RNA-seq] Kallisto</v>
       </c>
       <c r="B11" s="90" t="s">
@@ -21778,7 +21787,7 @@
     </row>
     <row r="12" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E12,"PharmaCompanyX_",""),"]-[",C12,"] ",D12)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[RNA-seq] Sailfish</v>
       </c>
       <c r="B12" s="90" t="s">
@@ -21812,7 +21821,7 @@
     </row>
     <row r="13" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E13,"PharmaCompanyX_",""),"]-[",C13,"] ",D13)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[RNA-seq] Salmon</v>
       </c>
       <c r="B13" s="90" t="s">
@@ -21846,7 +21855,7 @@
     </row>
     <row r="14" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E14,"PharmaCompanyX_",""),"]-[",C14,"] ",D14)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[RNA-seq] Tophat</v>
       </c>
       <c r="B14" s="90" t="s">
@@ -21880,7 +21889,7 @@
     </row>
     <row r="15" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E15,"PharmaCompanyX_",""),"]-[",C15,"] ",D15)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Fusion] Defuse</v>
       </c>
       <c r="B15" s="90" t="s">
@@ -21914,7 +21923,7 @@
     </row>
     <row r="16" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E16,"PharmaCompanyX_",""),"]-[",C16,"] ",D16)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Fusion] FusionCatcher</v>
       </c>
       <c r="B16" s="90" t="s">
@@ -21948,7 +21957,7 @@
     </row>
     <row r="17" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E17,"PharmaCompanyX_",""),"]-[",C17,"] ",D17)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Fusion] Tophat Fusion</v>
       </c>
       <c r="B17" s="90" t="s">
@@ -21982,7 +21991,7 @@
     </row>
     <row r="18" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E18,"PharmaCompanyX_",""),"]-[",C18,"] ",D18)</f>
+        <f t="shared" si="0"/>
         <v>[external]-[Fusion] custom pipeline - Foundation Medicine</v>
       </c>
       <c r="B18" s="90" t="s">
@@ -22016,7 +22025,7 @@
     </row>
     <row r="19" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E19,"PharmaCompanyX_",""),"]-[",C19,"] ",D19)</f>
+        <f t="shared" si="0"/>
         <v>[Affymetrix]-[Microarray] Affymetrix Bioconductor CDF v3.2.0</v>
       </c>
       <c r="B19" s="90" t="s">
@@ -22054,7 +22063,7 @@
     </row>
     <row r="20" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E20,"PharmaCompanyX_",""),"]-[",C20,"] ",D20)</f>
+        <f t="shared" si="0"/>
         <v>[Affymetrix]-[Microarray] UMich Alt CDF v20.0.0</v>
       </c>
       <c r="B20" s="90" t="s">
@@ -22092,7 +22101,7 @@
     </row>
     <row r="21" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E21,"PharmaCompanyX_",""),"]-[",IF(L21=FALSE,"Custom: ",""),F21,IF(ISBLANK(G21),"",CONCATENATE(" ",G21)),"] ",D21)</f>
+        <f t="shared" ref="A21:A30" si="1">CONCATENATE("[",SUBSTITUTE(E21,"PharmaCompanyX_",""),"]-[",IF(L21=FALSE,"Custom: ",""),F21,IF(ISBLANK(G21),"",CONCATENATE(" ",G21)),"] ",D21)</f>
         <v>[DNAnexus]-[RNAseq_Expression_AlignmentBased v1.3.3] Cufflinks</v>
       </c>
       <c r="B21" s="90" t="s">
@@ -22130,7 +22139,7 @@
     </row>
     <row r="22" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E22,"PharmaCompanyX_",""),"]-[",IF(L22=FALSE,"Custom: ",""),F22,IF(ISBLANK(G22),"",CONCATENATE(" ",G22)),"] ",D22)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[RNAseq_Expression_AlignmentBased v1.3.3] RSEM</v>
       </c>
       <c r="B22" s="90" t="s">
@@ -22168,7 +22177,7 @@
     </row>
     <row r="23" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E23,"PharmaCompanyX_",""),"]-[",IF(L23=FALSE,"Custom: ",""),F23,IF(ISBLANK(G23),"",CONCATENATE(" ",G23)),"] ",D23)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[RNAseq_Expression_AlignmentFree v2.0.0] Salmon</v>
       </c>
       <c r="B23" s="90" t="s">
@@ -22206,7 +22215,7 @@
     </row>
     <row r="24" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E24,"PharmaCompanyX_",""),"]-[",IF(L24=FALSE,"Custom: ",""),F24,IF(ISBLANK(G24),"",CONCATENATE(" ",G24)),"] ",D24)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[HLA_Typing v0.1] HLAreporter - Exome-seq</v>
       </c>
       <c r="B24" s="90" t="s">
@@ -22244,7 +22253,7 @@
     </row>
     <row r="25" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E25,"PharmaCompanyX_",""),"]-[",IF(L25=FALSE,"Custom: ",""),F25,IF(ISBLANK(G25),"",CONCATENATE(" ",G25)),"] ",D25)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[RNAseq_Fusion v2.0.0] Tophat Fusion</v>
       </c>
       <c r="B25" s="90" t="s">
@@ -22282,7 +22291,7 @@
     </row>
     <row r="26" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E26,"PharmaCompanyX_",""),"]-[",IF(L26=FALSE,"Custom: ",""),F26,IF(ISBLANK(G26),"",CONCATENATE(" ",G26)),"] ",D26)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[RNAseq_Fusion v2.0.0] Defuse</v>
       </c>
       <c r="B26" s="90" t="s">
@@ -22320,7 +22329,7 @@
     </row>
     <row r="27" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E27,"PharmaCompanyX_",""),"]-[",IF(L27=FALSE,"Custom: ",""),F27,IF(ISBLANK(G27),"",CONCATENATE(" ",G27)),"] ",D27)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[RNAseq_Fusion v2.0.0] FusionCatcher</v>
       </c>
       <c r="B27" s="90" t="s">
@@ -22358,7 +22367,7 @@
     </row>
     <row r="28" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E28,"PharmaCompanyX_",""),"]-[",IF(L28=FALSE,"Custom: ",""),F28,IF(ISBLANK(G28),"",CONCATENATE(" ",G28)),"] ",D28)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[DNAseq_TumorNormal v1.4.2] Mutect / SnpEff / GEMINI / Indels</v>
       </c>
       <c r="B28" s="90" t="s">
@@ -22398,7 +22407,7 @@
     </row>
     <row r="29" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E29,"PharmaCompanyX_",""),"]-[",IF(L29=FALSE,"Custom: ",""),F29,IF(ISBLANK(G29),"",CONCATENATE(" ",G29)),"] ",D29)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[DNAseq_TumorOnly v1.4.2] Mutect / SnpEff / GEMINI / Indels</v>
       </c>
       <c r="B29" s="90" t="s">
@@ -22438,7 +22447,7 @@
     </row>
     <row r="30" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="87" t="str">
-        <f>CONCATENATE("[",SUBSTITUTE(E30,"PharmaCompanyX_",""),"]-[",IF(L30=FALSE,"Custom: ",""),F30,IF(ISBLANK(G30),"",CONCATENATE(" ",G30)),"] ",D30)</f>
+        <f t="shared" si="1"/>
         <v>[DNAnexus]-[Variant_Annotation v0.3] SnpEff / GEMINI</v>
       </c>
       <c r="B30" s="90" t="s">

</xml_diff>

<commit_message>
update excel template with update pipeline names
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_sample.xlsx
+++ b/inst/extdata/scidb_metadata_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/revealgenomics/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D466A4-4BF6-1A4A-94AE-AA72EF1440B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8C643F-3F0F-604E-B952-6D6C12945567}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4600" yWindow="1580" windowWidth="28780" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,14 @@
     <sheet name="featureset_choices" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -168,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="565">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1109,9 +1117,6 @@
     <t>Pipelines</t>
   </si>
   <si>
-    <t>[external]-[Single Nucleotide Variant] custom pipeline - Foundation Medicine</t>
-  </si>
-  <si>
     <t>DNA - mutations - custom filter - external collaborator</t>
   </si>
   <si>
@@ -1124,15 +1129,9 @@
     <t>variant_fusion_cnv__fmi.txt</t>
   </si>
   <si>
-    <t>[external]-[Fusion] custom pipeline - Foundation Medicine</t>
-  </si>
-  <si>
     <t>gene - counts</t>
   </si>
   <si>
-    <t>[external]-[Exome CNV] custom pipeline - Foundation Medicine</t>
-  </si>
-  <si>
     <t>DNA - copy number value - custom filter - external partner</t>
   </si>
   <si>
@@ -1190,12 +1189,6 @@
     <t>HMM - hidden Markov model</t>
   </si>
   <si>
-    <t>custom pipeline - Foundation Medicine</t>
-  </si>
-  <si>
-    <t>external workflow (Foundation Medicine)</t>
-  </si>
-  <si>
     <t>Whole Genome CNV</t>
   </si>
   <si>
@@ -1884,6 +1877,24 @@
   </si>
   <si>
     <t>PharmaCompanyX-S3</t>
+  </si>
+  <si>
+    <t>[external]-[Targeted Region CNV] FoundationOne Heme (FMI)</t>
+  </si>
+  <si>
+    <t>[external]-[Fusion] FoundationOne Heme (FMI)</t>
+  </si>
+  <si>
+    <t>[external]-[Single Nucleotide Variant] Targeted Region - FoundationOne Heme (FMI)</t>
+  </si>
+  <si>
+    <t>Targeted Region - FoundationOne Heme (FMI)</t>
+  </si>
+  <si>
+    <t>FoundationOne Heme (FMI)</t>
+  </si>
+  <si>
+    <t>Targeted Region CNV</t>
   </si>
 </sst>
 </file>
@@ -2652,7 +2663,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -2987,7 +2998,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3309,7 +3320,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -3476,7 +3487,7 @@
           <a:effectLst/>
           <a:extLst>
             <a:ext uri="{C572A759-6A51-4108-AA02-DFA0A04FC94B}">
-              <ma14:wrappingTextBoxFlag xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" val="1"/>
+              <ma14:wrappingTextBoxFlag xmlns:ma14="http://schemas.microsoft.com/office/mac/drawingml/2011/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" val="1"/>
             </a:ext>
           </a:extLst>
         </xdr:spPr>
@@ -5055,7 +5066,7 @@
     </row>
     <row r="21" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -5066,12 +5077,12 @@
         <v>5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -5082,12 +5093,12 @@
         <v>5</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -5098,12 +5109,12 @@
         <v>5</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -5114,7 +5125,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -5189,20 +5200,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="94" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F2" s="26"/>
       <c r="G2" s="25" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H2" s="24" t="b">
         <v>1</v>
@@ -5218,20 +5229,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="94" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="11" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="H3" s="32" t="b">
         <v>1</v>
@@ -5247,20 +5258,20 @@
         <v>3</v>
       </c>
       <c r="B4" s="94" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="11" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H4" s="32" t="b">
         <v>1</v>
@@ -5275,20 +5286,20 @@
         <v>15</v>
       </c>
       <c r="B5" s="94" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="11" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H5" s="32" t="b">
         <v>1</v>
@@ -5304,20 +5315,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="94" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="11" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H6" s="32" t="b">
         <v>1</v>
@@ -5333,20 +5344,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="11" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H7" s="32" t="b">
         <v>1</v>
@@ -5362,20 +5373,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C8" s="44" t="s">
+        <v>416</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>421</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>426</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="11" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H8" s="32" t="b">
         <v>1</v>
@@ -5391,20 +5402,20 @@
         <v>7</v>
       </c>
       <c r="B9" s="94" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="11" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H9" s="32" t="b">
         <v>1</v>
@@ -5420,20 +5431,20 @@
         <v>8</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="11" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H10" s="32" t="b">
         <v>1</v>
@@ -5449,20 +5460,20 @@
         <v>9</v>
       </c>
       <c r="B11" s="94" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="C11" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H11" s="32" t="b">
         <v>1</v>
@@ -5478,22 +5489,22 @@
         <v>10</v>
       </c>
       <c r="B12" s="94" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="C12" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H12" s="32" t="b">
         <v>1</v>
@@ -5509,22 +5520,22 @@
         <v>11</v>
       </c>
       <c r="B13" s="94" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="C13" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H13" s="32" t="b">
         <v>1</v>
@@ -5539,22 +5550,22 @@
         <v>32</v>
       </c>
       <c r="B14" s="94" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C14" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H14" s="32" t="b">
         <v>0</v>
@@ -5570,22 +5581,22 @@
         <v>12</v>
       </c>
       <c r="B15" s="94" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C15" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H15" s="32" t="b">
         <v>0</v>
@@ -5601,22 +5612,22 @@
         <v>13</v>
       </c>
       <c r="B16" s="94" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="C16" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H16" s="32" t="b">
         <v>0</v>
@@ -5632,22 +5643,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="94" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C17" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H17" s="32" t="b">
         <v>0</v>
@@ -5662,20 +5673,20 @@
         <v>16</v>
       </c>
       <c r="B18" s="94" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C18" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H18" s="32" t="b">
         <v>0</v>
@@ -5690,20 +5701,20 @@
         <v>17</v>
       </c>
       <c r="B19" s="94" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C19" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H19" s="32" t="b">
         <v>0</v>
@@ -5718,20 +5729,20 @@
         <v>20</v>
       </c>
       <c r="B20" s="94" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C20" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H20" s="32" t="b">
         <v>1</v>
@@ -5746,20 +5757,20 @@
         <v>21</v>
       </c>
       <c r="B21" s="94" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C21" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H21" s="32" t="b">
         <v>0</v>
@@ -5774,20 +5785,20 @@
         <v>22</v>
       </c>
       <c r="B22" s="94" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="C22" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H22" s="32" t="b">
         <v>0</v>
@@ -5802,20 +5813,20 @@
         <v>23</v>
       </c>
       <c r="B23" s="94" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C23" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H23" s="32" t="b">
         <v>0</v>
@@ -5830,22 +5841,22 @@
         <v>24</v>
       </c>
       <c r="B24" s="94" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="C24" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H24" s="32" t="b">
         <v>1</v>
@@ -5860,22 +5871,22 @@
         <v>25</v>
       </c>
       <c r="B25" s="94" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C25" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H25" s="32" t="b">
         <v>1</v>
@@ -5890,20 +5901,20 @@
         <v>26</v>
       </c>
       <c r="B26" s="94" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C26" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H26" s="32" t="b">
         <v>1</v>
@@ -5918,20 +5929,20 @@
         <v>27</v>
       </c>
       <c r="B27" s="94" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C27" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H27" s="32" t="b">
         <v>0</v>
@@ -5946,20 +5957,20 @@
         <v>28</v>
       </c>
       <c r="B28" s="94" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C28" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H28" s="32" t="b">
         <v>0</v>
@@ -5974,22 +5985,22 @@
         <v>29</v>
       </c>
       <c r="B29" s="94" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C29" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H29" s="32" t="b">
         <v>0</v>
@@ -6004,22 +6015,22 @@
         <v>30</v>
       </c>
       <c r="B30" s="94" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="C30" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H30" s="32" t="b">
         <v>1</v>
@@ -6034,22 +6045,22 @@
         <v>31</v>
       </c>
       <c r="B31" s="94" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="C31" s="44" t="s">
         <v>285</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H31" s="32" t="b">
         <v>1</v>
@@ -6064,7 +6075,7 @@
         <v>999</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -6205,33 +6216,33 @@
     </row>
     <row r="2" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>166</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D3" s="32">
         <v>37</v>
@@ -6243,16 +6254,16 @@
     </row>
     <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>166</v>
@@ -6261,33 +6272,33 @@
     </row>
     <row r="5" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>166</v>
       </c>
       <c r="F5" s="96" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D6" s="32">
         <v>38</v>
@@ -6299,13 +6310,13 @@
     </row>
     <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D7" s="32">
         <v>38</v>
@@ -6317,16 +6328,16 @@
     </row>
     <row r="8" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>166</v>
@@ -6335,16 +6346,16 @@
     </row>
     <row r="9" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>166</v>
@@ -6353,16 +6364,16 @@
     </row>
     <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>166</v>
@@ -6371,16 +6382,16 @@
     </row>
     <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>166</v>
@@ -6389,16 +6400,16 @@
     </row>
     <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>166</v>
@@ -6407,16 +6418,16 @@
     </row>
     <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>166</v>
@@ -6425,16 +6436,16 @@
     </row>
     <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>166</v>
@@ -6443,16 +6454,16 @@
     </row>
     <row r="15" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>166</v>
@@ -6461,16 +6472,16 @@
     </row>
     <row r="16" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>166</v>
@@ -6479,16 +6490,16 @@
     </row>
     <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>166</v>
@@ -6497,16 +6508,16 @@
     </row>
     <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>166</v>
@@ -6515,16 +6526,16 @@
     </row>
     <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>166</v>
@@ -6533,16 +6544,16 @@
     </row>
     <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>166</v>
@@ -6551,16 +6562,16 @@
     </row>
     <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>166</v>
@@ -6569,16 +6580,16 @@
     </row>
     <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>166</v>
@@ -6587,16 +6598,16 @@
     </row>
     <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>166</v>
@@ -6605,16 +6616,16 @@
     </row>
     <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>166</v>
@@ -6623,16 +6634,16 @@
     </row>
     <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>166</v>
@@ -6641,16 +6652,16 @@
     </row>
     <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>166</v>
@@ -6659,16 +6670,16 @@
     </row>
     <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>166</v>
@@ -6677,13 +6688,13 @@
     </row>
     <row r="28" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D28" s="32">
         <v>37</v>
@@ -6695,13 +6706,13 @@
     </row>
     <row r="29" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D29" s="32">
         <v>38</v>
@@ -7660,10 +7671,10 @@
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="29" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="F15" s="30">
         <v>1</v>
@@ -7722,7 +7733,7 @@
         <v>62</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="F16" s="30">
         <v>5</v>
@@ -14340,7 +14351,7 @@
         <v>251</v>
       </c>
       <c r="O2" s="25" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="P2" s="25" t="s">
         <v>252</v>
@@ -14401,7 +14412,7 @@
         <v>251</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>259</v>
@@ -20424,8 +20435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:IV19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20508,25 +20519,25 @@
         <v>283</v>
       </c>
       <c r="F2" s="63" t="s">
+        <v>561</v>
+      </c>
+      <c r="G2" s="57" t="s">
         <v>305</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>306</v>
       </c>
       <c r="H2" s="64">
         <v>999</v>
       </c>
       <c r="I2" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J2" s="57" t="s">
         <v>307</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>308</v>
       </c>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
       <c r="N2" s="66" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20547,25 +20558,25 @@
         <v>292</v>
       </c>
       <c r="F3" s="63" t="s">
+        <v>561</v>
+      </c>
+      <c r="G3" s="44" t="s">
         <v>305</v>
-      </c>
-      <c r="G3" s="44" t="s">
-        <v>306</v>
       </c>
       <c r="H3" s="48">
         <v>999</v>
       </c>
       <c r="I3" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J3" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20586,25 +20597,25 @@
         <v>294</v>
       </c>
       <c r="F4" s="63" t="s">
+        <v>561</v>
+      </c>
+      <c r="G4" s="44" t="s">
         <v>305</v>
-      </c>
-      <c r="G4" s="44" t="s">
-        <v>306</v>
       </c>
       <c r="H4" s="48">
         <v>999</v>
       </c>
       <c r="I4" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J4" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J4" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20625,25 +20636,25 @@
         <v>283</v>
       </c>
       <c r="F5" s="68" t="s">
-        <v>310</v>
+        <v>560</v>
       </c>
       <c r="G5" s="44" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H5" s="48">
         <v>999</v>
       </c>
       <c r="I5" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J5" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J5" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20664,25 +20675,25 @@
         <v>292</v>
       </c>
       <c r="F6" s="68" t="s">
-        <v>310</v>
+        <v>560</v>
       </c>
       <c r="G6" s="44" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H6" s="48">
         <v>999</v>
       </c>
       <c r="I6" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J6" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J6" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20703,25 +20714,25 @@
         <v>294</v>
       </c>
       <c r="F7" s="68" t="s">
-        <v>310</v>
+        <v>560</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H7" s="48">
         <v>999</v>
       </c>
       <c r="I7" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J7" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J7" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20742,25 +20753,25 @@
         <v>283</v>
       </c>
       <c r="F8" s="65" t="s">
-        <v>312</v>
+        <v>559</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H8" s="48">
         <v>999</v>
       </c>
       <c r="I8" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J8" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J8" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20781,25 +20792,25 @@
         <v>292</v>
       </c>
       <c r="F9" s="65" t="s">
-        <v>312</v>
+        <v>559</v>
       </c>
       <c r="G9" s="44" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H9" s="48">
         <v>999</v>
       </c>
       <c r="I9" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J9" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J9" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20820,25 +20831,25 @@
         <v>294</v>
       </c>
       <c r="F10" s="65" t="s">
-        <v>312</v>
+        <v>559</v>
       </c>
       <c r="G10" s="44" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H10" s="48">
         <v>999</v>
       </c>
       <c r="I10" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J10" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J10" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20859,25 +20870,25 @@
         <v>295</v>
       </c>
       <c r="F11" s="65" t="s">
-        <v>312</v>
+        <v>559</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H11" s="48">
         <v>999</v>
       </c>
       <c r="I11" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J11" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J11" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20898,25 +20909,25 @@
         <v>283</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H12" s="48">
         <v>2</v>
       </c>
       <c r="I12" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J12" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J12" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="67" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20937,25 +20948,25 @@
         <v>295</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H13" s="48">
         <v>2</v>
       </c>
       <c r="I13" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J13" s="44" t="s">
         <v>307</v>
-      </c>
-      <c r="J13" s="44" t="s">
-        <v>308</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="67" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -20976,25 +20987,25 @@
         <v>296</v>
       </c>
       <c r="F14" s="70" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G14" s="70" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H14" s="71">
         <v>2</v>
       </c>
       <c r="I14" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="J14" s="40" t="s">
         <v>307</v>
-      </c>
-      <c r="J14" s="40" t="s">
-        <v>308</v>
       </c>
       <c r="K14" s="72"/>
       <c r="L14" s="72"/>
       <c r="M14" s="72"/>
       <c r="N14" s="73" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -21015,25 +21026,25 @@
         <v>299</v>
       </c>
       <c r="F15" s="76" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G15" s="63" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H15" s="75">
         <v>1</v>
       </c>
       <c r="I15" s="77" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K15" s="78"/>
       <c r="L15" s="78"/>
       <c r="M15" s="78"/>
       <c r="N15" s="79" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -21054,25 +21065,25 @@
         <v>302</v>
       </c>
       <c r="F16" s="76" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G16" s="57" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H16" s="24">
         <v>1</v>
       </c>
       <c r="I16" s="66" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
       <c r="M16" s="26"/>
       <c r="N16" s="66" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -21093,25 +21104,25 @@
         <v>303</v>
       </c>
       <c r="F17" s="76" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G17" s="44" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H17" s="32">
         <v>1</v>
       </c>
       <c r="I17" s="67" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="67" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -21132,25 +21143,25 @@
         <v>299</v>
       </c>
       <c r="F18" s="68" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G18" s="44" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H18" s="32">
         <v>2</v>
       </c>
       <c r="I18" s="67" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="67" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -21171,25 +21182,25 @@
         <v>302</v>
       </c>
       <c r="F19" s="80" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G19" s="44" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H19" s="32">
         <v>2</v>
       </c>
       <c r="I19" s="67" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="67" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -21376,8 +21387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:IV34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -21441,19 +21452,19 @@
         <v>[external]-[Exome CNV] CBS - Circular Binary Segmentation</v>
       </c>
       <c r="B2" s="88" t="s">
+        <v>322</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>323</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="E2" s="66" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="F2" s="66" t="s">
         <v>326</v>
-      </c>
-      <c r="D2" s="66" t="s">
-        <v>327</v>
-      </c>
-      <c r="E2" s="66" t="s">
-        <v>328</v>
-      </c>
-      <c r="F2" s="66" t="s">
-        <v>329</v>
       </c>
       <c r="G2" s="89"/>
       <c r="H2" s="23" t="b">
@@ -21468,7 +21479,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="66" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -21477,19 +21488,19 @@
         <v>[external]-[Exome CNV] HMM - hidden Markov model</v>
       </c>
       <c r="B3" s="90" t="s">
+        <v>322</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>323</v>
+      </c>
+      <c r="D3" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="E3" s="67" t="s">
         <v>325</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="F3" s="67" t="s">
         <v>326</v>
-      </c>
-      <c r="D3" s="67" t="s">
-        <v>331</v>
-      </c>
-      <c r="E3" s="67" t="s">
-        <v>328</v>
-      </c>
-      <c r="F3" s="67" t="s">
-        <v>329</v>
       </c>
       <c r="G3" s="38"/>
       <c r="H3" s="31" t="b">
@@ -21504,28 +21515,28 @@
         <v>0</v>
       </c>
       <c r="M3" s="67" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="87" t="str">
         <f t="shared" si="0"/>
-        <v>[external]-[Exome CNV] custom pipeline - Foundation Medicine</v>
+        <v>[external]-[Targeted Region CNV] FoundationOne Heme (FMI)</v>
       </c>
       <c r="B4" s="90" t="s">
+        <v>322</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>564</v>
+      </c>
+      <c r="D4" s="67" t="s">
+        <v>563</v>
+      </c>
+      <c r="E4" s="67" t="s">
         <v>325</v>
       </c>
-      <c r="C4" s="67" t="s">
-        <v>326</v>
-      </c>
-      <c r="D4" s="67" t="s">
-        <v>332</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>328</v>
-      </c>
       <c r="F4" s="67" t="s">
-        <v>333</v>
+        <v>563</v>
       </c>
       <c r="G4" s="38"/>
       <c r="H4" s="31" t="b">
@@ -21547,19 +21558,19 @@
         <v>[external]-[Whole Genome CNV] CBS - Circular Binary Segmentation</v>
       </c>
       <c r="B5" s="90" t="s">
+        <v>322</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>329</v>
+      </c>
+      <c r="D5" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="E5" s="67" t="s">
         <v>325</v>
       </c>
-      <c r="C5" s="67" t="s">
-        <v>334</v>
-      </c>
-      <c r="D5" s="67" t="s">
-        <v>327</v>
-      </c>
-      <c r="E5" s="67" t="s">
-        <v>328</v>
-      </c>
       <c r="F5" s="67" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="G5" s="38"/>
       <c r="H5" s="31" t="b">
@@ -21574,7 +21585,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="67" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -21583,19 +21594,19 @@
         <v>[external]-[Whole Genome CNV] HMM - hidden Markov model</v>
       </c>
       <c r="B6" s="90" t="s">
+        <v>322</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>329</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>328</v>
+      </c>
+      <c r="E6" s="67" t="s">
         <v>325</v>
       </c>
-      <c r="C6" s="67" t="s">
-        <v>334</v>
-      </c>
-      <c r="D6" s="67" t="s">
-        <v>331</v>
-      </c>
-      <c r="E6" s="67" t="s">
-        <v>328</v>
-      </c>
       <c r="F6" s="67" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="G6" s="38"/>
       <c r="H6" s="31" t="b">
@@ -21610,7 +21621,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="67" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -21619,19 +21630,19 @@
         <v>[external]-[Single Nucleotide Variant] MuTect / seurat / strelka</v>
       </c>
       <c r="B7" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C7" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D7" s="67" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F7" s="67" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G7" s="38"/>
       <c r="H7" s="31" t="b">
@@ -21650,22 +21661,22 @@
     <row r="8" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="87" t="str">
         <f t="shared" si="0"/>
-        <v>[external]-[Single Nucleotide Variant] custom pipeline - Foundation Medicine</v>
+        <v>[external]-[Single Nucleotide Variant] Targeted Region - FoundationOne Heme (FMI)</v>
       </c>
       <c r="B8" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D8" s="67" t="s">
-        <v>332</v>
+        <v>562</v>
       </c>
       <c r="E8" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F8" s="67" t="s">
-        <v>333</v>
+        <v>562</v>
       </c>
       <c r="G8" s="38"/>
       <c r="H8" s="31" t="b">
@@ -21680,7 +21691,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="67" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -21689,19 +21700,19 @@
         <v>[external]-[RNA-seq] Cufflinks</v>
       </c>
       <c r="B9" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D9" s="67" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E9" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F9" s="67" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="G9" s="38"/>
       <c r="H9" s="31" t="b">
@@ -21723,19 +21734,19 @@
         <v>[external]-[RNA-seq] HTSeq</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D10" s="67" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E10" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F10" s="67" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G10" s="38"/>
       <c r="H10" s="31" t="b">
@@ -21757,19 +21768,19 @@
         <v>[external]-[RNA-seq] Kallisto</v>
       </c>
       <c r="B11" s="90" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>337</v>
+      </c>
+      <c r="D11" s="67" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="67" t="s">
-        <v>342</v>
-      </c>
-      <c r="D11" s="67" t="s">
-        <v>346</v>
-      </c>
       <c r="E11" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F11" s="67" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="31" t="b">
@@ -21791,19 +21802,19 @@
         <v>[external]-[RNA-seq] Sailfish</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C12" s="67" t="s">
+        <v>337</v>
+      </c>
+      <c r="D12" s="67" t="s">
         <v>342</v>
       </c>
-      <c r="D12" s="67" t="s">
-        <v>347</v>
-      </c>
       <c r="E12" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F12" s="67" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="G12" s="38"/>
       <c r="H12" s="31" t="b">
@@ -21825,19 +21836,19 @@
         <v>[external]-[RNA-seq] Salmon</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D13" s="67" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F13" s="67" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G13" s="38"/>
       <c r="H13" s="31" t="b">
@@ -21859,19 +21870,19 @@
         <v>[external]-[RNA-seq] Tophat</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C14" s="67" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D14" s="67" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E14" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F14" s="67" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="G14" s="38"/>
       <c r="H14" s="31" t="b">
@@ -21893,19 +21904,19 @@
         <v>[external]-[Fusion] Defuse</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C15" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D15" s="67" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F15" s="67" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="G15" s="38"/>
       <c r="H15" s="31" t="b">
@@ -21927,19 +21938,19 @@
         <v>[external]-[Fusion] FusionCatcher</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F16" s="67" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="31" t="b">
@@ -21961,19 +21972,19 @@
         <v>[external]-[Fusion] Tophat Fusion</v>
       </c>
       <c r="B17" s="90" t="s">
+        <v>345</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>346</v>
+      </c>
+      <c r="D17" s="67" t="s">
         <v>350</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="E17" s="67" t="s">
+        <v>325</v>
+      </c>
+      <c r="F17" s="67" t="s">
         <v>351</v>
-      </c>
-      <c r="D17" s="67" t="s">
-        <v>355</v>
-      </c>
-      <c r="E17" s="67" t="s">
-        <v>328</v>
-      </c>
-      <c r="F17" s="67" t="s">
-        <v>356</v>
       </c>
       <c r="G17" s="38"/>
       <c r="H17" s="31" t="b">
@@ -21992,22 +22003,22 @@
     <row r="18" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="87" t="str">
         <f t="shared" si="0"/>
-        <v>[external]-[Fusion] custom pipeline - Foundation Medicine</v>
+        <v>[external]-[Fusion] FoundationOne Heme (FMI)</v>
       </c>
       <c r="B18" s="90" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D18" s="67" t="s">
-        <v>332</v>
+        <v>563</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F18" s="67" t="s">
-        <v>333</v>
+        <v>563</v>
       </c>
       <c r="G18" s="38"/>
       <c r="H18" s="31" t="b">
@@ -22029,29 +22040,29 @@
         <v>[Affymetrix]-[Microarray] Affymetrix Bioconductor CDF v3.2.0</v>
       </c>
       <c r="B19" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D19" s="67" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G19" s="67" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="H19" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I19" s="38"/>
       <c r="J19" s="67" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="K19" s="31" t="b">
         <v>1</v>
@@ -22067,29 +22078,29 @@
         <v>[Affymetrix]-[Microarray] UMich Alt CDF v20.0.0</v>
       </c>
       <c r="B20" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C20" s="67" t="s">
+        <v>352</v>
+      </c>
+      <c r="D20" s="67" t="s">
         <v>357</v>
       </c>
-      <c r="D20" s="67" t="s">
-        <v>362</v>
-      </c>
       <c r="E20" s="67" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="F20" s="67" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="G20" s="67" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="H20" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I20" s="38"/>
       <c r="J20" s="67" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="K20" s="31" t="b">
         <v>1</v>
@@ -22105,29 +22116,29 @@
         <v>[DNAnexus]-[RNAseq_Expression_AlignmentBased v1.3.3] Cufflinks</v>
       </c>
       <c r="B21" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C21" s="67" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D21" s="67" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E21" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F21" s="91" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="G21" s="67" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="H21" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I21" s="38"/>
       <c r="J21" s="67" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="K21" s="31" t="b">
         <v>1</v>
@@ -22143,29 +22154,29 @@
         <v>[DNAnexus]-[RNAseq_Expression_AlignmentBased v1.3.3] RSEM</v>
       </c>
       <c r="B22" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C22" s="67" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D22" s="67" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="E22" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F22" s="91" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="G22" s="67" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="H22" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I22" s="38"/>
       <c r="J22" s="67" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="K22" s="31" t="b">
         <v>1</v>
@@ -22181,29 +22192,29 @@
         <v>[DNAnexus]-[RNAseq_Expression_AlignmentFree v2.0.0] Salmon</v>
       </c>
       <c r="B23" s="90" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C23" s="67" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D23" s="67" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E23" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F23" s="91" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="G23" s="67" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="H23" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I23" s="38"/>
       <c r="J23" s="67" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="K23" s="31" t="b">
         <v>1</v>
@@ -22219,29 +22230,29 @@
         <v>[DNAnexus]-[HLA_Typing v0.1] HLAreporter - Exome-seq</v>
       </c>
       <c r="B24" s="90" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F24" s="91" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G24" s="67" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="H24" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I24" s="38"/>
       <c r="J24" s="67" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="K24" s="31" t="b">
         <v>1</v>
@@ -22257,29 +22268,29 @@
         <v>[DNAnexus]-[RNAseq_Fusion v2.0.0] Tophat Fusion</v>
       </c>
       <c r="B25" s="90" t="s">
+        <v>345</v>
+      </c>
+      <c r="C25" s="67" t="s">
+        <v>346</v>
+      </c>
+      <c r="D25" s="67" t="s">
         <v>350</v>
       </c>
-      <c r="C25" s="67" t="s">
-        <v>351</v>
-      </c>
-      <c r="D25" s="67" t="s">
-        <v>355</v>
-      </c>
       <c r="E25" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F25" s="91" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G25" s="67" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="H25" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I25" s="38"/>
       <c r="J25" s="67" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="K25" s="31" t="b">
         <v>1</v>
@@ -22295,29 +22306,29 @@
         <v>[DNAnexus]-[RNAseq_Fusion v2.0.0] Defuse</v>
       </c>
       <c r="B26" s="90" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C26" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D26" s="67" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E26" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F26" s="91" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G26" s="67" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="H26" s="31" t="b">
         <v>0</v>
       </c>
       <c r="I26" s="38"/>
       <c r="J26" s="67" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="K26" s="31" t="b">
         <v>1</v>
@@ -22333,29 +22344,29 @@
         <v>[DNAnexus]-[RNAseq_Fusion v2.0.0] FusionCatcher</v>
       </c>
       <c r="B27" s="90" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C27" s="67" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E27" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F27" s="91" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G27" s="67" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="H27" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I27" s="38"/>
       <c r="J27" s="67" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="K27" s="31" t="b">
         <v>1</v>
@@ -22371,31 +22382,31 @@
         <v>[DNAnexus]-[DNAseq_TumorNormal v1.4.2] Mutect / SnpEff / GEMINI / Indels</v>
       </c>
       <c r="B28" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C28" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D28" s="67" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E28" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F28" s="91" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="G28" s="67" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="H28" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I28" s="67" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="J28" s="67" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="K28" s="31" t="b">
         <v>1</v>
@@ -22411,31 +22422,31 @@
         <v>[DNAnexus]-[DNAseq_TumorOnly v1.4.2] Mutect / SnpEff / GEMINI / Indels</v>
       </c>
       <c r="B29" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C29" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D29" s="67" t="s">
+        <v>375</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>550</v>
+      </c>
+      <c r="F29" s="91" t="s">
+        <v>379</v>
+      </c>
+      <c r="G29" s="67" t="s">
+        <v>377</v>
+      </c>
+      <c r="H29" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="67" t="s">
         <v>380</v>
       </c>
-      <c r="E29" s="67" t="s">
-        <v>555</v>
-      </c>
-      <c r="F29" s="91" t="s">
-        <v>384</v>
-      </c>
-      <c r="G29" s="67" t="s">
-        <v>382</v>
-      </c>
-      <c r="H29" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="67" t="s">
-        <v>385</v>
-      </c>
       <c r="J29" s="67" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="K29" s="31" t="b">
         <v>1</v>
@@ -22451,29 +22462,29 @@
         <v>[DNAnexus]-[Variant_Annotation v0.3] SnpEff / GEMINI</v>
       </c>
       <c r="B30" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C30" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D30" s="67" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E30" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F30" s="91" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="G30" s="67" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="H30" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I30" s="38"/>
       <c r="J30" s="67" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="K30" s="31" t="b">
         <v>1</v>
@@ -22489,29 +22500,29 @@
         <v>[DNAnexus]-[Variant_Custom: MuTect HC + PoN + Annotate] Mutect / SnpEff / GEMINI</v>
       </c>
       <c r="B31" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C31" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D31" s="67" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E31" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F31" s="67" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="G31" s="38"/>
       <c r="H31" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I31" s="67" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="J31" s="67" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="K31" s="31" t="b">
         <v>1</v>
@@ -22527,29 +22538,29 @@
         <v>[DNAnexus]-[Variant_Custom: GATK + Annotate] GATK / SnpEff / GEMINI</v>
       </c>
       <c r="B32" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C32" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D32" s="67" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E32" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F32" s="67" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="G32" s="38"/>
       <c r="H32" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I32" s="67" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="J32" s="67" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="K32" s="31" t="b">
         <v>1</v>
@@ -22565,29 +22576,29 @@
         <v>[DNAnexus]-[Variant_Custom: VarScan + Annotate] VarScan / SnpEff / GEMINI</v>
       </c>
       <c r="B33" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C33" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D33" s="67" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E33" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F33" s="67" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G33" s="38"/>
       <c r="H33" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I33" s="67" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="J33" s="67" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="K33" s="31" t="b">
         <v>1</v>
@@ -22603,31 +22614,31 @@
         <v>[DNAnexus]-[Variant_DNA-seq Tumor Only v1.3] Mutect / SnpEff / GEMINI (non-TCGA gnomAD &amp; ExAC)</v>
       </c>
       <c r="B34" s="90" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C34" s="67" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D34" s="67" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="F34" s="91" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G34" s="67" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="H34" s="31" t="b">
         <v>1</v>
       </c>
       <c r="I34" s="67" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="J34" s="67" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="K34" s="31" t="b">
         <v>1</v>

</xml_diff>